<commit_message>
Fixed cognacy of 'north wind' units, updated measures accordingly
</commit_message>
<xml_diff>
--- a/Multilingual Cloze Tests/Distances/northwindsun_matched_words_annotated.xlsx
+++ b/Multilingual Cloze Tests/Distances/northwindsun_matched_words_annotated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phgeorgis/Documents/Work/HiWi/Multilingual Cloze Tests/Distances/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A96FBA5-9764-C94A-883F-EE0C6DA5CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E30638B-E1AF-1B47-AA00-437C7FC6CF0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16039" uniqueCount="960">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16015" uniqueCount="960">
   <si>
     <t>L1</t>
   </si>
@@ -3262,8 +3262,8 @@
   <dimension ref="A1:H2466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2310" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2327" sqref="M2327"/>
+      <pane ySplit="1" topLeftCell="A2321" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2340" sqref="M2340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -59950,7 +59950,7 @@
     </row>
     <row r="2322" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2322" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2322" t="s">
         <v>943</v>
@@ -59959,7 +59959,7 @@
         <v>944</v>
       </c>
       <c r="D2322" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="E2322" t="s">
         <v>945</v>
@@ -59968,7 +59968,7 @@
         <v>946</v>
       </c>
       <c r="G2322">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2322" t="s">
         <v>896</v>
@@ -59976,7 +59976,7 @@
     </row>
     <row r="2323" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2323" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="B2323" t="s">
         <v>943</v>
@@ -59985,7 +59985,7 @@
         <v>944</v>
       </c>
       <c r="D2323" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2323" t="s">
         <v>947</v>
@@ -59994,7 +59994,7 @@
         <v>948</v>
       </c>
       <c r="G2323">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2323" t="s">
         <v>896</v>
@@ -60002,7 +60002,7 @@
     </row>
     <row r="2324" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2324" t="s">
-        <v>299</v>
+        <v>7</v>
       </c>
       <c r="B2324" t="s">
         <v>943</v>
@@ -60011,7 +60011,7 @@
         <v>944</v>
       </c>
       <c r="D2324" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2324" t="s">
         <v>949</v>
@@ -60020,7 +60020,7 @@
         <v>950</v>
       </c>
       <c r="G2324">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2324" t="s">
         <v>896</v>
@@ -60028,7 +60028,7 @@
     </row>
     <row r="2325" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2325" t="s">
-        <v>395</v>
+        <v>7</v>
       </c>
       <c r="B2325" t="s">
         <v>943</v>
@@ -60037,7 +60037,7 @@
         <v>944</v>
       </c>
       <c r="D2325" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2325" t="s">
         <v>951</v>
@@ -60046,7 +60046,7 @@
         <v>397</v>
       </c>
       <c r="G2325">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2325" t="s">
         <v>896</v>
@@ -60054,7 +60054,7 @@
     </row>
     <row r="2326" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2326" t="s">
-        <v>480</v>
+        <v>7</v>
       </c>
       <c r="B2326" t="s">
         <v>943</v>
@@ -60063,7 +60063,7 @@
         <v>944</v>
       </c>
       <c r="D2326" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2326" t="s">
         <v>952</v>
@@ -60072,7 +60072,7 @@
         <v>482</v>
       </c>
       <c r="G2326">
-        <v>0.88235294099999995</v>
+        <v>0.88235300000000005</v>
       </c>
       <c r="H2326" t="s">
         <v>896</v>
@@ -60080,7 +60080,7 @@
     </row>
     <row r="2327" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2327" t="s">
-        <v>522</v>
+        <v>7</v>
       </c>
       <c r="B2327" t="s">
         <v>943</v>
@@ -60098,7 +60098,7 @@
         <v>954</v>
       </c>
       <c r="G2327">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2327" t="s">
         <v>896</v>
@@ -60106,7 +60106,7 @@
     </row>
     <row r="2328" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2328" t="s">
-        <v>603</v>
+        <v>7</v>
       </c>
       <c r="B2328" t="s">
         <v>943</v>
@@ -60115,7 +60115,7 @@
         <v>944</v>
       </c>
       <c r="D2328" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2328" t="s">
         <v>955</v>
@@ -60124,7 +60124,7 @@
         <v>956</v>
       </c>
       <c r="G2328">
-        <v>0.58823529399999996</v>
+        <v>0.58823499999999995</v>
       </c>
       <c r="H2328" t="s">
         <v>896</v>
@@ -60132,7 +60132,7 @@
     </row>
     <row r="2329" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2329" t="s">
-        <v>681</v>
+        <v>7</v>
       </c>
       <c r="B2329" t="s">
         <v>943</v>
@@ -60141,7 +60141,7 @@
         <v>944</v>
       </c>
       <c r="D2329" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2329" t="s">
         <v>957</v>
@@ -60150,7 +60150,7 @@
         <v>958</v>
       </c>
       <c r="G2329">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2329" t="s">
         <v>896</v>
@@ -60158,7 +60158,7 @@
     </row>
     <row r="2330" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2330" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B2330" t="s">
         <v>945</v>
@@ -60167,7 +60167,7 @@
         <v>946</v>
       </c>
       <c r="D2330" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2330" t="s">
         <v>947</v>
@@ -60176,7 +60176,7 @@
         <v>948</v>
       </c>
       <c r="G2330">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2330" t="s">
         <v>896</v>
@@ -60184,7 +60184,7 @@
     </row>
     <row r="2331" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2331" t="s">
-        <v>299</v>
+        <v>10</v>
       </c>
       <c r="B2331" t="s">
         <v>945</v>
@@ -60193,7 +60193,7 @@
         <v>946</v>
       </c>
       <c r="D2331" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2331" t="s">
         <v>949</v>
@@ -60202,7 +60202,7 @@
         <v>950</v>
       </c>
       <c r="G2331">
-        <v>0.53333333299999997</v>
+        <v>0.53333299999999995</v>
       </c>
       <c r="H2331" t="s">
         <v>896</v>
@@ -60210,7 +60210,7 @@
     </row>
     <row r="2332" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2332" t="s">
-        <v>395</v>
+        <v>10</v>
       </c>
       <c r="B2332" t="s">
         <v>945</v>
@@ -60219,7 +60219,7 @@
         <v>946</v>
       </c>
       <c r="D2332" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2332" t="s">
         <v>951</v>
@@ -60228,15 +60228,12 @@
         <v>397</v>
       </c>
       <c r="G2332">
-        <v>0.93333333299999999</v>
-      </c>
-      <c r="H2332" t="s">
-        <v>896</v>
+        <v>0.93333299999999997</v>
       </c>
     </row>
     <row r="2333" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2333" t="s">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="B2333" t="s">
         <v>945</v>
@@ -60245,7 +60242,7 @@
         <v>946</v>
       </c>
       <c r="D2333" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2333" t="s">
         <v>952</v>
@@ -60256,13 +60253,10 @@
       <c r="G2333">
         <v>1</v>
       </c>
-      <c r="H2333" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2334" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2334" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="B2334" t="s">
         <v>945</v>
@@ -60288,7 +60282,7 @@
     </row>
     <row r="2335" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2335" t="s">
-        <v>603</v>
+        <v>10</v>
       </c>
       <c r="B2335" t="s">
         <v>945</v>
@@ -60297,7 +60291,7 @@
         <v>946</v>
       </c>
       <c r="D2335" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2335" t="s">
         <v>955</v>
@@ -60314,7 +60308,7 @@
     </row>
     <row r="2336" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2336" t="s">
-        <v>681</v>
+        <v>10</v>
       </c>
       <c r="B2336" t="s">
         <v>945</v>
@@ -60323,7 +60317,7 @@
         <v>946</v>
       </c>
       <c r="D2336" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2336" t="s">
         <v>957</v>
@@ -60340,7 +60334,7 @@
     </row>
     <row r="2337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2337" t="s">
-        <v>299</v>
+        <v>214</v>
       </c>
       <c r="B2337" t="s">
         <v>947</v>
@@ -60349,7 +60343,7 @@
         <v>948</v>
       </c>
       <c r="D2337" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2337" t="s">
         <v>949</v>
@@ -60358,7 +60352,7 @@
         <v>950</v>
       </c>
       <c r="G2337">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2337" t="s">
         <v>896</v>
@@ -60366,7 +60360,7 @@
     </row>
     <row r="2338" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2338" t="s">
-        <v>395</v>
+        <v>214</v>
       </c>
       <c r="B2338" t="s">
         <v>947</v>
@@ -60375,7 +60369,7 @@
         <v>948</v>
       </c>
       <c r="D2338" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2338" t="s">
         <v>951</v>
@@ -60386,13 +60380,10 @@
       <c r="G2338">
         <v>1</v>
       </c>
-      <c r="H2338" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2339" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2339" t="s">
-        <v>480</v>
+        <v>214</v>
       </c>
       <c r="B2339" t="s">
         <v>947</v>
@@ -60401,7 +60392,7 @@
         <v>948</v>
       </c>
       <c r="D2339" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2339" t="s">
         <v>952</v>
@@ -60410,15 +60401,12 @@
         <v>482</v>
       </c>
       <c r="G2339">
-        <v>0.94117647100000001</v>
-      </c>
-      <c r="H2339" t="s">
-        <v>896</v>
+        <v>0.94117600000000001</v>
       </c>
     </row>
     <row r="2340" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2340" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="B2340" t="s">
         <v>947</v>
@@ -60436,7 +60424,7 @@
         <v>954</v>
       </c>
       <c r="G2340">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2340" t="s">
         <v>896</v>
@@ -60444,7 +60432,7 @@
     </row>
     <row r="2341" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2341" t="s">
-        <v>603</v>
+        <v>214</v>
       </c>
       <c r="B2341" t="s">
         <v>947</v>
@@ -60453,7 +60441,7 @@
         <v>948</v>
       </c>
       <c r="D2341" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2341" t="s">
         <v>955</v>
@@ -60462,7 +60450,7 @@
         <v>956</v>
       </c>
       <c r="G2341">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2341" t="s">
         <v>896</v>
@@ -60470,7 +60458,7 @@
     </row>
     <row r="2342" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2342" t="s">
-        <v>681</v>
+        <v>214</v>
       </c>
       <c r="B2342" t="s">
         <v>947</v>
@@ -60479,7 +60467,7 @@
         <v>948</v>
       </c>
       <c r="D2342" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2342" t="s">
         <v>957</v>
@@ -60488,7 +60476,7 @@
         <v>958</v>
       </c>
       <c r="G2342">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2342" t="s">
         <v>896</v>
@@ -60496,7 +60484,7 @@
     </row>
     <row r="2343" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2343" t="s">
-        <v>395</v>
+        <v>299</v>
       </c>
       <c r="B2343" t="s">
         <v>949</v>
@@ -60505,7 +60493,7 @@
         <v>950</v>
       </c>
       <c r="D2343" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2343" t="s">
         <v>951</v>
@@ -60514,15 +60502,12 @@
         <v>397</v>
       </c>
       <c r="G2343">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2343" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2344" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2344" t="s">
-        <v>480</v>
+        <v>299</v>
       </c>
       <c r="B2344" t="s">
         <v>949</v>
@@ -60531,7 +60516,7 @@
         <v>950</v>
       </c>
       <c r="D2344" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2344" t="s">
         <v>952</v>
@@ -60540,15 +60525,12 @@
         <v>482</v>
       </c>
       <c r="G2344">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2344" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2345" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2345" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="B2345" t="s">
         <v>949</v>
@@ -60566,7 +60548,7 @@
         <v>954</v>
       </c>
       <c r="G2345">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2345" t="s">
         <v>896</v>
@@ -60574,7 +60556,7 @@
     </row>
     <row r="2346" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2346" t="s">
-        <v>603</v>
+        <v>299</v>
       </c>
       <c r="B2346" t="s">
         <v>949</v>
@@ -60583,7 +60565,7 @@
         <v>950</v>
       </c>
       <c r="D2346" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2346" t="s">
         <v>955</v>
@@ -60600,7 +60582,7 @@
     </row>
     <row r="2347" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2347" t="s">
-        <v>681</v>
+        <v>299</v>
       </c>
       <c r="B2347" t="s">
         <v>949</v>
@@ -60609,7 +60591,7 @@
         <v>950</v>
       </c>
       <c r="D2347" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2347" t="s">
         <v>957</v>
@@ -60626,7 +60608,7 @@
     </row>
     <row r="2348" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2348" t="s">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="B2348" t="s">
         <v>951</v>
@@ -60635,7 +60617,7 @@
         <v>397</v>
       </c>
       <c r="D2348" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2348" t="s">
         <v>952</v>
@@ -60652,7 +60634,7 @@
     </row>
     <row r="2349" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2349" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="B2349" t="s">
         <v>951</v>
@@ -60670,7 +60652,7 @@
         <v>954</v>
       </c>
       <c r="G2349">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2349" t="s">
         <v>896</v>
@@ -60678,7 +60660,7 @@
     </row>
     <row r="2350" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2350" t="s">
-        <v>603</v>
+        <v>395</v>
       </c>
       <c r="B2350" t="s">
         <v>951</v>
@@ -60687,7 +60669,7 @@
         <v>397</v>
       </c>
       <c r="D2350" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2350" t="s">
         <v>955</v>
@@ -60704,7 +60686,7 @@
     </row>
     <row r="2351" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2351" t="s">
-        <v>681</v>
+        <v>395</v>
       </c>
       <c r="B2351" t="s">
         <v>951</v>
@@ -60713,7 +60695,7 @@
         <v>397</v>
       </c>
       <c r="D2351" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2351" t="s">
         <v>957</v>
@@ -60730,7 +60712,7 @@
     </row>
     <row r="2352" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2352" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B2352" t="s">
         <v>952</v>
@@ -60748,7 +60730,7 @@
         <v>954</v>
       </c>
       <c r="G2352">
-        <v>0.78571428600000004</v>
+        <v>0.78571400000000002</v>
       </c>
       <c r="H2352" t="s">
         <v>896</v>
@@ -60756,7 +60738,7 @@
     </row>
     <row r="2353" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2353" t="s">
-        <v>603</v>
+        <v>480</v>
       </c>
       <c r="B2353" t="s">
         <v>952</v>
@@ -60765,7 +60747,7 @@
         <v>482</v>
       </c>
       <c r="D2353" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2353" t="s">
         <v>955</v>
@@ -60782,7 +60764,7 @@
     </row>
     <row r="2354" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2354" t="s">
-        <v>681</v>
+        <v>480</v>
       </c>
       <c r="B2354" t="s">
         <v>952</v>
@@ -60791,7 +60773,7 @@
         <v>482</v>
       </c>
       <c r="D2354" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2354" t="s">
         <v>957</v>
@@ -60808,7 +60790,7 @@
     </row>
     <row r="2355" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2355" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="B2355" t="s">
         <v>953</v>
@@ -60817,7 +60799,7 @@
         <v>954</v>
       </c>
       <c r="D2355" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2355" t="s">
         <v>955</v>
@@ -60834,7 +60816,7 @@
     </row>
     <row r="2356" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2356" t="s">
-        <v>681</v>
+        <v>522</v>
       </c>
       <c r="B2356" t="s">
         <v>953</v>
@@ -60843,7 +60825,7 @@
         <v>954</v>
       </c>
       <c r="D2356" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2356" t="s">
         <v>957</v>
@@ -60860,7 +60842,7 @@
     </row>
     <row r="2357" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2357" t="s">
-        <v>681</v>
+        <v>603</v>
       </c>
       <c r="B2357" t="s">
         <v>955</v>
@@ -60869,7 +60851,7 @@
         <v>956</v>
       </c>
       <c r="D2357" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2357" t="s">
         <v>957</v>
@@ -60886,7 +60868,7 @@
     </row>
     <row r="2358" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2358" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2358" t="s">
         <v>943</v>
@@ -60895,7 +60877,7 @@
         <v>944</v>
       </c>
       <c r="D2358" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="E2358" t="s">
         <v>945</v>
@@ -60904,7 +60886,7 @@
         <v>959</v>
       </c>
       <c r="G2358">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2358" t="s">
         <v>896</v>
@@ -60912,7 +60894,7 @@
     </row>
     <row r="2359" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2359" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="B2359" t="s">
         <v>943</v>
@@ -60921,7 +60903,7 @@
         <v>944</v>
       </c>
       <c r="D2359" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2359" t="s">
         <v>947</v>
@@ -60930,7 +60912,7 @@
         <v>948</v>
       </c>
       <c r="G2359">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2359" t="s">
         <v>896</v>
@@ -60938,7 +60920,7 @@
     </row>
     <row r="2360" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2360" t="s">
-        <v>299</v>
+        <v>7</v>
       </c>
       <c r="B2360" t="s">
         <v>943</v>
@@ -60947,7 +60929,7 @@
         <v>944</v>
       </c>
       <c r="D2360" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2360" t="s">
         <v>949</v>
@@ -60956,7 +60938,7 @@
         <v>950</v>
       </c>
       <c r="G2360">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2360" t="s">
         <v>896</v>
@@ -60964,7 +60946,7 @@
     </row>
     <row r="2361" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2361" t="s">
-        <v>395</v>
+        <v>7</v>
       </c>
       <c r="B2361" t="s">
         <v>943</v>
@@ -60973,7 +60955,7 @@
         <v>944</v>
       </c>
       <c r="D2361" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2361" t="s">
         <v>951</v>
@@ -60982,7 +60964,7 @@
         <v>397</v>
       </c>
       <c r="G2361">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2361" t="s">
         <v>896</v>
@@ -60990,7 +60972,7 @@
     </row>
     <row r="2362" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2362" t="s">
-        <v>480</v>
+        <v>7</v>
       </c>
       <c r="B2362" t="s">
         <v>943</v>
@@ -60999,7 +60981,7 @@
         <v>944</v>
       </c>
       <c r="D2362" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2362" t="s">
         <v>952</v>
@@ -61008,7 +60990,7 @@
         <v>482</v>
       </c>
       <c r="G2362">
-        <v>0.88235294099999995</v>
+        <v>0.88235300000000005</v>
       </c>
       <c r="H2362" t="s">
         <v>896</v>
@@ -61016,7 +60998,7 @@
     </row>
     <row r="2363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2363" t="s">
-        <v>522</v>
+        <v>7</v>
       </c>
       <c r="B2363" t="s">
         <v>943</v>
@@ -61034,7 +61016,7 @@
         <v>954</v>
       </c>
       <c r="G2363">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2363" t="s">
         <v>896</v>
@@ -61042,7 +61024,7 @@
     </row>
     <row r="2364" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2364" t="s">
-        <v>603</v>
+        <v>7</v>
       </c>
       <c r="B2364" t="s">
         <v>943</v>
@@ -61051,7 +61033,7 @@
         <v>944</v>
       </c>
       <c r="D2364" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2364" t="s">
         <v>955</v>
@@ -61060,7 +61042,7 @@
         <v>956</v>
       </c>
       <c r="G2364">
-        <v>0.58823529399999996</v>
+        <v>0.58823499999999995</v>
       </c>
       <c r="H2364" t="s">
         <v>896</v>
@@ -61068,7 +61050,7 @@
     </row>
     <row r="2365" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2365" t="s">
-        <v>681</v>
+        <v>7</v>
       </c>
       <c r="B2365" t="s">
         <v>943</v>
@@ -61077,7 +61059,7 @@
         <v>944</v>
       </c>
       <c r="D2365" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2365" t="s">
         <v>957</v>
@@ -61086,7 +61068,7 @@
         <v>958</v>
       </c>
       <c r="G2365">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2365" t="s">
         <v>896</v>
@@ -61094,7 +61076,7 @@
     </row>
     <row r="2366" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2366" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B2366" t="s">
         <v>945</v>
@@ -61103,7 +61085,7 @@
         <v>959</v>
       </c>
       <c r="D2366" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2366" t="s">
         <v>947</v>
@@ -61112,7 +61094,7 @@
         <v>948</v>
       </c>
       <c r="G2366">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2366" t="s">
         <v>896</v>
@@ -61120,7 +61102,7 @@
     </row>
     <row r="2367" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2367" t="s">
-        <v>299</v>
+        <v>10</v>
       </c>
       <c r="B2367" t="s">
         <v>945</v>
@@ -61129,7 +61111,7 @@
         <v>959</v>
       </c>
       <c r="D2367" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2367" t="s">
         <v>949</v>
@@ -61138,7 +61120,7 @@
         <v>950</v>
       </c>
       <c r="G2367">
-        <v>0.53333333299999997</v>
+        <v>0.53333299999999995</v>
       </c>
       <c r="H2367" t="s">
         <v>896</v>
@@ -61146,7 +61128,7 @@
     </row>
     <row r="2368" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2368" t="s">
-        <v>395</v>
+        <v>10</v>
       </c>
       <c r="B2368" t="s">
         <v>945</v>
@@ -61155,7 +61137,7 @@
         <v>959</v>
       </c>
       <c r="D2368" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2368" t="s">
         <v>951</v>
@@ -61164,15 +61146,12 @@
         <v>397</v>
       </c>
       <c r="G2368">
-        <v>0.93333333299999999</v>
-      </c>
-      <c r="H2368" t="s">
-        <v>896</v>
+        <v>0.93333299999999997</v>
       </c>
     </row>
     <row r="2369" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2369" t="s">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="B2369" t="s">
         <v>945</v>
@@ -61181,7 +61160,7 @@
         <v>959</v>
       </c>
       <c r="D2369" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2369" t="s">
         <v>952</v>
@@ -61192,13 +61171,10 @@
       <c r="G2369">
         <v>1</v>
       </c>
-      <c r="H2369" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2370" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2370" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="B2370" t="s">
         <v>945</v>
@@ -61224,7 +61200,7 @@
     </row>
     <row r="2371" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2371" t="s">
-        <v>603</v>
+        <v>10</v>
       </c>
       <c r="B2371" t="s">
         <v>945</v>
@@ -61233,7 +61209,7 @@
         <v>959</v>
       </c>
       <c r="D2371" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2371" t="s">
         <v>955</v>
@@ -61250,7 +61226,7 @@
     </row>
     <row r="2372" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2372" t="s">
-        <v>681</v>
+        <v>10</v>
       </c>
       <c r="B2372" t="s">
         <v>945</v>
@@ -61259,7 +61235,7 @@
         <v>959</v>
       </c>
       <c r="D2372" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2372" t="s">
         <v>957</v>
@@ -61276,7 +61252,7 @@
     </row>
     <row r="2373" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2373" t="s">
-        <v>299</v>
+        <v>214</v>
       </c>
       <c r="B2373" t="s">
         <v>947</v>
@@ -61285,7 +61261,7 @@
         <v>948</v>
       </c>
       <c r="D2373" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2373" t="s">
         <v>949</v>
@@ -61294,7 +61270,7 @@
         <v>950</v>
       </c>
       <c r="G2373">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2373" t="s">
         <v>896</v>
@@ -61302,7 +61278,7 @@
     </row>
     <row r="2374" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2374" t="s">
-        <v>395</v>
+        <v>214</v>
       </c>
       <c r="B2374" t="s">
         <v>947</v>
@@ -61311,7 +61287,7 @@
         <v>948</v>
       </c>
       <c r="D2374" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2374" t="s">
         <v>951</v>
@@ -61322,13 +61298,10 @@
       <c r="G2374">
         <v>1</v>
       </c>
-      <c r="H2374" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2375" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2375" t="s">
-        <v>480</v>
+        <v>214</v>
       </c>
       <c r="B2375" t="s">
         <v>947</v>
@@ -61337,7 +61310,7 @@
         <v>948</v>
       </c>
       <c r="D2375" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2375" t="s">
         <v>952</v>
@@ -61346,15 +61319,12 @@
         <v>482</v>
       </c>
       <c r="G2375">
-        <v>0.94117647100000001</v>
-      </c>
-      <c r="H2375" t="s">
-        <v>896</v>
+        <v>0.94117600000000001</v>
       </c>
     </row>
     <row r="2376" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2376" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="B2376" t="s">
         <v>947</v>
@@ -61372,7 +61342,7 @@
         <v>954</v>
       </c>
       <c r="G2376">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2376" t="s">
         <v>896</v>
@@ -61380,7 +61350,7 @@
     </row>
     <row r="2377" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2377" t="s">
-        <v>603</v>
+        <v>214</v>
       </c>
       <c r="B2377" t="s">
         <v>947</v>
@@ -61389,7 +61359,7 @@
         <v>948</v>
       </c>
       <c r="D2377" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2377" t="s">
         <v>955</v>
@@ -61398,7 +61368,7 @@
         <v>956</v>
       </c>
       <c r="G2377">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2377" t="s">
         <v>896</v>
@@ -61406,7 +61376,7 @@
     </row>
     <row r="2378" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2378" t="s">
-        <v>681</v>
+        <v>214</v>
       </c>
       <c r="B2378" t="s">
         <v>947</v>
@@ -61415,7 +61385,7 @@
         <v>948</v>
       </c>
       <c r="D2378" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2378" t="s">
         <v>957</v>
@@ -61424,7 +61394,7 @@
         <v>958</v>
       </c>
       <c r="G2378">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2378" t="s">
         <v>896</v>
@@ -61432,7 +61402,7 @@
     </row>
     <row r="2379" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2379" t="s">
-        <v>395</v>
+        <v>299</v>
       </c>
       <c r="B2379" t="s">
         <v>949</v>
@@ -61441,7 +61411,7 @@
         <v>950</v>
       </c>
       <c r="D2379" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2379" t="s">
         <v>951</v>
@@ -61450,15 +61420,12 @@
         <v>397</v>
       </c>
       <c r="G2379">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2379" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2380" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2380" t="s">
-        <v>480</v>
+        <v>299</v>
       </c>
       <c r="B2380" t="s">
         <v>949</v>
@@ -61467,7 +61434,7 @@
         <v>950</v>
       </c>
       <c r="D2380" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2380" t="s">
         <v>952</v>
@@ -61476,15 +61443,12 @@
         <v>482</v>
       </c>
       <c r="G2380">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2380" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2381" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2381" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="B2381" t="s">
         <v>949</v>
@@ -61502,7 +61466,7 @@
         <v>954</v>
       </c>
       <c r="G2381">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2381" t="s">
         <v>896</v>
@@ -61510,7 +61474,7 @@
     </row>
     <row r="2382" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2382" t="s">
-        <v>603</v>
+        <v>299</v>
       </c>
       <c r="B2382" t="s">
         <v>949</v>
@@ -61519,7 +61483,7 @@
         <v>950</v>
       </c>
       <c r="D2382" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2382" t="s">
         <v>955</v>
@@ -61536,7 +61500,7 @@
     </row>
     <row r="2383" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2383" t="s">
-        <v>681</v>
+        <v>299</v>
       </c>
       <c r="B2383" t="s">
         <v>949</v>
@@ -61545,7 +61509,7 @@
         <v>950</v>
       </c>
       <c r="D2383" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2383" t="s">
         <v>957</v>
@@ -61562,7 +61526,7 @@
     </row>
     <row r="2384" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2384" t="s">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="B2384" t="s">
         <v>951</v>
@@ -61571,7 +61535,7 @@
         <v>397</v>
       </c>
       <c r="D2384" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2384" t="s">
         <v>952</v>
@@ -61588,7 +61552,7 @@
     </row>
     <row r="2385" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2385" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="B2385" t="s">
         <v>951</v>
@@ -61606,7 +61570,7 @@
         <v>954</v>
       </c>
       <c r="G2385">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2385" t="s">
         <v>896</v>
@@ -61614,7 +61578,7 @@
     </row>
     <row r="2386" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2386" t="s">
-        <v>603</v>
+        <v>395</v>
       </c>
       <c r="B2386" t="s">
         <v>951</v>
@@ -61623,7 +61587,7 @@
         <v>397</v>
       </c>
       <c r="D2386" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2386" t="s">
         <v>955</v>
@@ -61640,7 +61604,7 @@
     </row>
     <row r="2387" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2387" t="s">
-        <v>681</v>
+        <v>395</v>
       </c>
       <c r="B2387" t="s">
         <v>951</v>
@@ -61649,7 +61613,7 @@
         <v>397</v>
       </c>
       <c r="D2387" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2387" t="s">
         <v>957</v>
@@ -61666,7 +61630,7 @@
     </row>
     <row r="2388" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2388" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B2388" t="s">
         <v>952</v>
@@ -61684,7 +61648,7 @@
         <v>954</v>
       </c>
       <c r="G2388">
-        <v>0.78571428600000004</v>
+        <v>0.78571400000000002</v>
       </c>
       <c r="H2388" t="s">
         <v>896</v>
@@ -61692,7 +61656,7 @@
     </row>
     <row r="2389" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2389" t="s">
-        <v>603</v>
+        <v>480</v>
       </c>
       <c r="B2389" t="s">
         <v>952</v>
@@ -61701,7 +61665,7 @@
         <v>482</v>
       </c>
       <c r="D2389" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2389" t="s">
         <v>955</v>
@@ -61718,7 +61682,7 @@
     </row>
     <row r="2390" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2390" t="s">
-        <v>681</v>
+        <v>480</v>
       </c>
       <c r="B2390" t="s">
         <v>952</v>
@@ -61727,7 +61691,7 @@
         <v>482</v>
       </c>
       <c r="D2390" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2390" t="s">
         <v>957</v>
@@ -61744,7 +61708,7 @@
     </row>
     <row r="2391" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2391" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="B2391" t="s">
         <v>953</v>
@@ -61753,7 +61717,7 @@
         <v>954</v>
       </c>
       <c r="D2391" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2391" t="s">
         <v>955</v>
@@ -61770,7 +61734,7 @@
     </row>
     <row r="2392" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2392" t="s">
-        <v>681</v>
+        <v>522</v>
       </c>
       <c r="B2392" t="s">
         <v>953</v>
@@ -61779,7 +61743,7 @@
         <v>954</v>
       </c>
       <c r="D2392" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2392" t="s">
         <v>957</v>
@@ -61796,7 +61760,7 @@
     </row>
     <row r="2393" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2393" t="s">
-        <v>681</v>
+        <v>603</v>
       </c>
       <c r="B2393" t="s">
         <v>955</v>
@@ -61805,7 +61769,7 @@
         <v>956</v>
       </c>
       <c r="D2393" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2393" t="s">
         <v>957</v>
@@ -61822,7 +61786,7 @@
     </row>
     <row r="2394" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2394" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2394" t="s">
         <v>943</v>
@@ -61831,7 +61795,7 @@
         <v>944</v>
       </c>
       <c r="D2394" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="E2394" t="s">
         <v>945</v>
@@ -61840,7 +61804,7 @@
         <v>946</v>
       </c>
       <c r="G2394">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2394" t="s">
         <v>896</v>
@@ -61848,7 +61812,7 @@
     </row>
     <row r="2395" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2395" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="B2395" t="s">
         <v>943</v>
@@ -61857,7 +61821,7 @@
         <v>944</v>
       </c>
       <c r="D2395" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2395" t="s">
         <v>947</v>
@@ -61866,7 +61830,7 @@
         <v>948</v>
       </c>
       <c r="G2395">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2395" t="s">
         <v>896</v>
@@ -61874,7 +61838,7 @@
     </row>
     <row r="2396" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2396" t="s">
-        <v>299</v>
+        <v>7</v>
       </c>
       <c r="B2396" t="s">
         <v>943</v>
@@ -61883,7 +61847,7 @@
         <v>944</v>
       </c>
       <c r="D2396" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2396" t="s">
         <v>949</v>
@@ -61892,7 +61856,7 @@
         <v>950</v>
       </c>
       <c r="G2396">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2396" t="s">
         <v>896</v>
@@ -61900,7 +61864,7 @@
     </row>
     <row r="2397" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2397" t="s">
-        <v>395</v>
+        <v>7</v>
       </c>
       <c r="B2397" t="s">
         <v>943</v>
@@ -61909,7 +61873,7 @@
         <v>944</v>
       </c>
       <c r="D2397" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2397" t="s">
         <v>951</v>
@@ -61918,7 +61882,7 @@
         <v>397</v>
       </c>
       <c r="G2397">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2397" t="s">
         <v>896</v>
@@ -61926,7 +61890,7 @@
     </row>
     <row r="2398" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2398" t="s">
-        <v>480</v>
+        <v>7</v>
       </c>
       <c r="B2398" t="s">
         <v>943</v>
@@ -61935,7 +61899,7 @@
         <v>944</v>
       </c>
       <c r="D2398" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2398" t="s">
         <v>952</v>
@@ -61944,7 +61908,7 @@
         <v>511</v>
       </c>
       <c r="G2398">
-        <v>0.88235294099999995</v>
+        <v>0.88235300000000005</v>
       </c>
       <c r="H2398" t="s">
         <v>896</v>
@@ -61952,7 +61916,7 @@
     </row>
     <row r="2399" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2399" t="s">
-        <v>522</v>
+        <v>7</v>
       </c>
       <c r="B2399" t="s">
         <v>943</v>
@@ -61970,7 +61934,7 @@
         <v>954</v>
       </c>
       <c r="G2399">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2399" t="s">
         <v>896</v>
@@ -61978,7 +61942,7 @@
     </row>
     <row r="2400" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2400" t="s">
-        <v>603</v>
+        <v>7</v>
       </c>
       <c r="B2400" t="s">
         <v>943</v>
@@ -61987,7 +61951,7 @@
         <v>944</v>
       </c>
       <c r="D2400" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2400" t="s">
         <v>955</v>
@@ -61996,7 +61960,7 @@
         <v>956</v>
       </c>
       <c r="G2400">
-        <v>0.58823529399999996</v>
+        <v>0.58823499999999995</v>
       </c>
       <c r="H2400" t="s">
         <v>896</v>
@@ -62004,7 +61968,7 @@
     </row>
     <row r="2401" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2401" t="s">
-        <v>681</v>
+        <v>7</v>
       </c>
       <c r="B2401" t="s">
         <v>943</v>
@@ -62013,7 +61977,7 @@
         <v>944</v>
       </c>
       <c r="D2401" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2401" t="s">
         <v>957</v>
@@ -62022,7 +61986,7 @@
         <v>958</v>
       </c>
       <c r="G2401">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2401" t="s">
         <v>896</v>
@@ -62030,7 +61994,7 @@
     </row>
     <row r="2402" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2402" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B2402" t="s">
         <v>945</v>
@@ -62039,7 +62003,7 @@
         <v>946</v>
       </c>
       <c r="D2402" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2402" t="s">
         <v>947</v>
@@ -62048,7 +62012,7 @@
         <v>948</v>
       </c>
       <c r="G2402">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2402" t="s">
         <v>896</v>
@@ -62056,7 +62020,7 @@
     </row>
     <row r="2403" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2403" t="s">
-        <v>299</v>
+        <v>10</v>
       </c>
       <c r="B2403" t="s">
         <v>945</v>
@@ -62065,7 +62029,7 @@
         <v>946</v>
       </c>
       <c r="D2403" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2403" t="s">
         <v>949</v>
@@ -62074,7 +62038,7 @@
         <v>950</v>
       </c>
       <c r="G2403">
-        <v>0.53333333299999997</v>
+        <v>0.53333299999999995</v>
       </c>
       <c r="H2403" t="s">
         <v>896</v>
@@ -62082,7 +62046,7 @@
     </row>
     <row r="2404" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2404" t="s">
-        <v>395</v>
+        <v>10</v>
       </c>
       <c r="B2404" t="s">
         <v>945</v>
@@ -62091,7 +62055,7 @@
         <v>946</v>
       </c>
       <c r="D2404" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2404" t="s">
         <v>951</v>
@@ -62100,15 +62064,12 @@
         <v>397</v>
       </c>
       <c r="G2404">
-        <v>0.93333333299999999</v>
-      </c>
-      <c r="H2404" t="s">
-        <v>896</v>
+        <v>0.93333299999999997</v>
       </c>
     </row>
     <row r="2405" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2405" t="s">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="B2405" t="s">
         <v>945</v>
@@ -62117,7 +62078,7 @@
         <v>946</v>
       </c>
       <c r="D2405" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2405" t="s">
         <v>952</v>
@@ -62128,13 +62089,10 @@
       <c r="G2405">
         <v>1</v>
       </c>
-      <c r="H2405" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2406" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2406" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="B2406" t="s">
         <v>945</v>
@@ -62160,7 +62118,7 @@
     </row>
     <row r="2407" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2407" t="s">
-        <v>603</v>
+        <v>10</v>
       </c>
       <c r="B2407" t="s">
         <v>945</v>
@@ -62169,7 +62127,7 @@
         <v>946</v>
       </c>
       <c r="D2407" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2407" t="s">
         <v>955</v>
@@ -62186,7 +62144,7 @@
     </row>
     <row r="2408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2408" t="s">
-        <v>681</v>
+        <v>10</v>
       </c>
       <c r="B2408" t="s">
         <v>945</v>
@@ -62195,7 +62153,7 @@
         <v>946</v>
       </c>
       <c r="D2408" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2408" t="s">
         <v>957</v>
@@ -62212,7 +62170,7 @@
     </row>
     <row r="2409" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2409" t="s">
-        <v>299</v>
+        <v>214</v>
       </c>
       <c r="B2409" t="s">
         <v>947</v>
@@ -62221,7 +62179,7 @@
         <v>948</v>
       </c>
       <c r="D2409" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2409" t="s">
         <v>949</v>
@@ -62230,7 +62188,7 @@
         <v>950</v>
       </c>
       <c r="G2409">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2409" t="s">
         <v>896</v>
@@ -62238,7 +62196,7 @@
     </row>
     <row r="2410" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2410" t="s">
-        <v>395</v>
+        <v>214</v>
       </c>
       <c r="B2410" t="s">
         <v>947</v>
@@ -62247,7 +62205,7 @@
         <v>948</v>
       </c>
       <c r="D2410" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2410" t="s">
         <v>951</v>
@@ -62258,13 +62216,10 @@
       <c r="G2410">
         <v>1</v>
       </c>
-      <c r="H2410" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2411" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2411" t="s">
-        <v>480</v>
+        <v>214</v>
       </c>
       <c r="B2411" t="s">
         <v>947</v>
@@ -62273,7 +62228,7 @@
         <v>948</v>
       </c>
       <c r="D2411" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2411" t="s">
         <v>952</v>
@@ -62282,15 +62237,12 @@
         <v>511</v>
       </c>
       <c r="G2411">
-        <v>0.94117647100000001</v>
-      </c>
-      <c r="H2411" t="s">
-        <v>896</v>
+        <v>0.94117600000000001</v>
       </c>
     </row>
     <row r="2412" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2412" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="B2412" t="s">
         <v>947</v>
@@ -62308,7 +62260,7 @@
         <v>954</v>
       </c>
       <c r="G2412">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2412" t="s">
         <v>896</v>
@@ -62316,7 +62268,7 @@
     </row>
     <row r="2413" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2413" t="s">
-        <v>603</v>
+        <v>214</v>
       </c>
       <c r="B2413" t="s">
         <v>947</v>
@@ -62325,7 +62277,7 @@
         <v>948</v>
       </c>
       <c r="D2413" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2413" t="s">
         <v>955</v>
@@ -62334,7 +62286,7 @@
         <v>956</v>
       </c>
       <c r="G2413">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2413" t="s">
         <v>896</v>
@@ -62342,7 +62294,7 @@
     </row>
     <row r="2414" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2414" t="s">
-        <v>681</v>
+        <v>214</v>
       </c>
       <c r="B2414" t="s">
         <v>947</v>
@@ -62351,7 +62303,7 @@
         <v>948</v>
       </c>
       <c r="D2414" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2414" t="s">
         <v>957</v>
@@ -62360,7 +62312,7 @@
         <v>958</v>
       </c>
       <c r="G2414">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2414" t="s">
         <v>896</v>
@@ -62368,7 +62320,7 @@
     </row>
     <row r="2415" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2415" t="s">
-        <v>395</v>
+        <v>299</v>
       </c>
       <c r="B2415" t="s">
         <v>949</v>
@@ -62377,7 +62329,7 @@
         <v>950</v>
       </c>
       <c r="D2415" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2415" t="s">
         <v>951</v>
@@ -62386,15 +62338,12 @@
         <v>397</v>
       </c>
       <c r="G2415">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2415" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2416" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2416" t="s">
-        <v>480</v>
+        <v>299</v>
       </c>
       <c r="B2416" t="s">
         <v>949</v>
@@ -62403,7 +62352,7 @@
         <v>950</v>
       </c>
       <c r="D2416" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2416" t="s">
         <v>952</v>
@@ -62412,15 +62361,12 @@
         <v>511</v>
       </c>
       <c r="G2416">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2416" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2417" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2417" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="B2417" t="s">
         <v>949</v>
@@ -62438,7 +62384,7 @@
         <v>954</v>
       </c>
       <c r="G2417">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2417" t="s">
         <v>896</v>
@@ -62446,7 +62392,7 @@
     </row>
     <row r="2418" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2418" t="s">
-        <v>603</v>
+        <v>299</v>
       </c>
       <c r="B2418" t="s">
         <v>949</v>
@@ -62455,7 +62401,7 @@
         <v>950</v>
       </c>
       <c r="D2418" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2418" t="s">
         <v>955</v>
@@ -62472,7 +62418,7 @@
     </row>
     <row r="2419" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2419" t="s">
-        <v>681</v>
+        <v>299</v>
       </c>
       <c r="B2419" t="s">
         <v>949</v>
@@ -62481,7 +62427,7 @@
         <v>950</v>
       </c>
       <c r="D2419" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2419" t="s">
         <v>957</v>
@@ -62498,7 +62444,7 @@
     </row>
     <row r="2420" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2420" t="s">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="B2420" t="s">
         <v>951</v>
@@ -62507,7 +62453,7 @@
         <v>397</v>
       </c>
       <c r="D2420" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2420" t="s">
         <v>952</v>
@@ -62524,7 +62470,7 @@
     </row>
     <row r="2421" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2421" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="B2421" t="s">
         <v>951</v>
@@ -62542,7 +62488,7 @@
         <v>954</v>
       </c>
       <c r="G2421">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2421" t="s">
         <v>896</v>
@@ -62550,7 +62496,7 @@
     </row>
     <row r="2422" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2422" t="s">
-        <v>603</v>
+        <v>395</v>
       </c>
       <c r="B2422" t="s">
         <v>951</v>
@@ -62559,7 +62505,7 @@
         <v>397</v>
       </c>
       <c r="D2422" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2422" t="s">
         <v>955</v>
@@ -62576,7 +62522,7 @@
     </row>
     <row r="2423" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2423" t="s">
-        <v>681</v>
+        <v>395</v>
       </c>
       <c r="B2423" t="s">
         <v>951</v>
@@ -62585,7 +62531,7 @@
         <v>397</v>
       </c>
       <c r="D2423" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2423" t="s">
         <v>957</v>
@@ -62602,7 +62548,7 @@
     </row>
     <row r="2424" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2424" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B2424" t="s">
         <v>952</v>
@@ -62620,7 +62566,7 @@
         <v>954</v>
       </c>
       <c r="G2424">
-        <v>0.78571428600000004</v>
+        <v>0.78571400000000002</v>
       </c>
       <c r="H2424" t="s">
         <v>896</v>
@@ -62628,7 +62574,7 @@
     </row>
     <row r="2425" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2425" t="s">
-        <v>603</v>
+        <v>480</v>
       </c>
       <c r="B2425" t="s">
         <v>952</v>
@@ -62637,7 +62583,7 @@
         <v>511</v>
       </c>
       <c r="D2425" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2425" t="s">
         <v>955</v>
@@ -62654,7 +62600,7 @@
     </row>
     <row r="2426" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2426" t="s">
-        <v>681</v>
+        <v>480</v>
       </c>
       <c r="B2426" t="s">
         <v>952</v>
@@ -62663,7 +62609,7 @@
         <v>511</v>
       </c>
       <c r="D2426" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2426" t="s">
         <v>957</v>
@@ -62680,7 +62626,7 @@
     </row>
     <row r="2427" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2427" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="B2427" t="s">
         <v>953</v>
@@ -62689,7 +62635,7 @@
         <v>954</v>
       </c>
       <c r="D2427" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2427" t="s">
         <v>955</v>
@@ -62706,7 +62652,7 @@
     </row>
     <row r="2428" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2428" t="s">
-        <v>681</v>
+        <v>522</v>
       </c>
       <c r="B2428" t="s">
         <v>953</v>
@@ -62715,7 +62661,7 @@
         <v>954</v>
       </c>
       <c r="D2428" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2428" t="s">
         <v>957</v>
@@ -62732,7 +62678,7 @@
     </row>
     <row r="2429" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2429" t="s">
-        <v>681</v>
+        <v>603</v>
       </c>
       <c r="B2429" t="s">
         <v>955</v>
@@ -62741,7 +62687,7 @@
         <v>956</v>
       </c>
       <c r="D2429" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2429" t="s">
         <v>957</v>
@@ -62758,7 +62704,7 @@
     </row>
     <row r="2430" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2430" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2430" t="s">
         <v>943</v>
@@ -62767,7 +62713,7 @@
         <v>944</v>
       </c>
       <c r="D2430" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="E2430" t="s">
         <v>945</v>
@@ -62776,7 +62722,7 @@
         <v>946</v>
       </c>
       <c r="G2430">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2430" t="s">
         <v>896</v>
@@ -62784,7 +62730,7 @@
     </row>
     <row r="2431" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2431" t="s">
-        <v>214</v>
+        <v>7</v>
       </c>
       <c r="B2431" t="s">
         <v>943</v>
@@ -62793,7 +62739,7 @@
         <v>944</v>
       </c>
       <c r="D2431" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2431" t="s">
         <v>947</v>
@@ -62802,7 +62748,7 @@
         <v>948</v>
       </c>
       <c r="G2431">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2431" t="s">
         <v>896</v>
@@ -62810,7 +62756,7 @@
     </row>
     <row r="2432" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2432" t="s">
-        <v>299</v>
+        <v>7</v>
       </c>
       <c r="B2432" t="s">
         <v>943</v>
@@ -62819,7 +62765,7 @@
         <v>944</v>
       </c>
       <c r="D2432" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2432" t="s">
         <v>949</v>
@@ -62828,7 +62774,7 @@
         <v>950</v>
       </c>
       <c r="G2432">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2432" t="s">
         <v>896</v>
@@ -62836,7 +62782,7 @@
     </row>
     <row r="2433" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2433" t="s">
-        <v>395</v>
+        <v>7</v>
       </c>
       <c r="B2433" t="s">
         <v>943</v>
@@ -62845,7 +62791,7 @@
         <v>944</v>
       </c>
       <c r="D2433" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2433" t="s">
         <v>951</v>
@@ -62854,7 +62800,7 @@
         <v>397</v>
       </c>
       <c r="G2433">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2433" t="s">
         <v>896</v>
@@ -62862,7 +62808,7 @@
     </row>
     <row r="2434" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2434" t="s">
-        <v>480</v>
+        <v>7</v>
       </c>
       <c r="B2434" t="s">
         <v>943</v>
@@ -62871,7 +62817,7 @@
         <v>944</v>
       </c>
       <c r="D2434" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2434" t="s">
         <v>952</v>
@@ -62880,7 +62826,7 @@
         <v>482</v>
       </c>
       <c r="G2434">
-        <v>0.88235294099999995</v>
+        <v>0.88235300000000005</v>
       </c>
       <c r="H2434" t="s">
         <v>896</v>
@@ -62888,7 +62834,7 @@
     </row>
     <row r="2435" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2435" t="s">
-        <v>522</v>
+        <v>7</v>
       </c>
       <c r="B2435" t="s">
         <v>943</v>
@@ -62906,7 +62852,7 @@
         <v>954</v>
       </c>
       <c r="G2435">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2435" t="s">
         <v>896</v>
@@ -62914,7 +62860,7 @@
     </row>
     <row r="2436" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2436" t="s">
-        <v>603</v>
+        <v>7</v>
       </c>
       <c r="B2436" t="s">
         <v>943</v>
@@ -62923,7 +62869,7 @@
         <v>944</v>
       </c>
       <c r="D2436" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2436" t="s">
         <v>955</v>
@@ -62932,7 +62878,7 @@
         <v>956</v>
       </c>
       <c r="G2436">
-        <v>0.58823529399999996</v>
+        <v>0.58823499999999995</v>
       </c>
       <c r="H2436" t="s">
         <v>896</v>
@@ -62940,7 +62886,7 @@
     </row>
     <row r="2437" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2437" t="s">
-        <v>681</v>
+        <v>7</v>
       </c>
       <c r="B2437" t="s">
         <v>943</v>
@@ -62949,7 +62895,7 @@
         <v>944</v>
       </c>
       <c r="D2437" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2437" t="s">
         <v>957</v>
@@ -62958,7 +62904,7 @@
         <v>958</v>
       </c>
       <c r="G2437">
-        <v>0.64705882400000003</v>
+        <v>0.64705900000000005</v>
       </c>
       <c r="H2437" t="s">
         <v>896</v>
@@ -62966,7 +62912,7 @@
     </row>
     <row r="2438" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2438" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B2438" t="s">
         <v>945</v>
@@ -62975,7 +62921,7 @@
         <v>946</v>
       </c>
       <c r="D2438" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="E2438" t="s">
         <v>947</v>
@@ -62984,7 +62930,7 @@
         <v>948</v>
       </c>
       <c r="G2438">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2438" t="s">
         <v>896</v>
@@ -62992,7 +62938,7 @@
     </row>
     <row r="2439" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2439" t="s">
-        <v>299</v>
+        <v>10</v>
       </c>
       <c r="B2439" t="s">
         <v>945</v>
@@ -63001,7 +62947,7 @@
         <v>946</v>
       </c>
       <c r="D2439" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2439" t="s">
         <v>949</v>
@@ -63010,7 +62956,7 @@
         <v>950</v>
       </c>
       <c r="G2439">
-        <v>0.53333333299999997</v>
+        <v>0.53333299999999995</v>
       </c>
       <c r="H2439" t="s">
         <v>896</v>
@@ -63018,7 +62964,7 @@
     </row>
     <row r="2440" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2440" t="s">
-        <v>395</v>
+        <v>10</v>
       </c>
       <c r="B2440" t="s">
         <v>945</v>
@@ -63027,7 +62973,7 @@
         <v>946</v>
       </c>
       <c r="D2440" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2440" t="s">
         <v>951</v>
@@ -63036,15 +62982,12 @@
         <v>397</v>
       </c>
       <c r="G2440">
-        <v>0.93333333299999999</v>
-      </c>
-      <c r="H2440" t="s">
-        <v>896</v>
+        <v>0.93333299999999997</v>
       </c>
     </row>
     <row r="2441" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2441" t="s">
-        <v>480</v>
+        <v>10</v>
       </c>
       <c r="B2441" t="s">
         <v>945</v>
@@ -63053,7 +62996,7 @@
         <v>946</v>
       </c>
       <c r="D2441" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2441" t="s">
         <v>952</v>
@@ -63064,13 +63007,10 @@
       <c r="G2441">
         <v>1</v>
       </c>
-      <c r="H2441" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2442" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2442" t="s">
-        <v>522</v>
+        <v>10</v>
       </c>
       <c r="B2442" t="s">
         <v>945</v>
@@ -63096,7 +63036,7 @@
     </row>
     <row r="2443" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2443" t="s">
-        <v>603</v>
+        <v>10</v>
       </c>
       <c r="B2443" t="s">
         <v>945</v>
@@ -63105,7 +63045,7 @@
         <v>946</v>
       </c>
       <c r="D2443" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2443" t="s">
         <v>955</v>
@@ -63122,7 +63062,7 @@
     </row>
     <row r="2444" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2444" t="s">
-        <v>681</v>
+        <v>10</v>
       </c>
       <c r="B2444" t="s">
         <v>945</v>
@@ -63131,7 +63071,7 @@
         <v>946</v>
       </c>
       <c r="D2444" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2444" t="s">
         <v>957</v>
@@ -63148,7 +63088,7 @@
     </row>
     <row r="2445" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2445" t="s">
-        <v>299</v>
+        <v>214</v>
       </c>
       <c r="B2445" t="s">
         <v>947</v>
@@ -63157,7 +63097,7 @@
         <v>948</v>
       </c>
       <c r="D2445" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="E2445" t="s">
         <v>949</v>
@@ -63166,7 +63106,7 @@
         <v>950</v>
       </c>
       <c r="G2445">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2445" t="s">
         <v>896</v>
@@ -63174,7 +63114,7 @@
     </row>
     <row r="2446" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2446" t="s">
-        <v>395</v>
+        <v>214</v>
       </c>
       <c r="B2446" t="s">
         <v>947</v>
@@ -63183,7 +63123,7 @@
         <v>948</v>
       </c>
       <c r="D2446" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2446" t="s">
         <v>951</v>
@@ -63194,13 +63134,10 @@
       <c r="G2446">
         <v>1</v>
       </c>
-      <c r="H2446" t="s">
-        <v>896</v>
-      </c>
     </row>
     <row r="2447" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2447" t="s">
-        <v>480</v>
+        <v>214</v>
       </c>
       <c r="B2447" t="s">
         <v>947</v>
@@ -63209,7 +63146,7 @@
         <v>948</v>
       </c>
       <c r="D2447" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2447" t="s">
         <v>952</v>
@@ -63218,15 +63155,12 @@
         <v>482</v>
       </c>
       <c r="G2447">
-        <v>0.94117647100000001</v>
-      </c>
-      <c r="H2447" t="s">
-        <v>896</v>
+        <v>0.94117600000000001</v>
       </c>
     </row>
     <row r="2448" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2448" t="s">
-        <v>522</v>
+        <v>214</v>
       </c>
       <c r="B2448" t="s">
         <v>947</v>
@@ -63244,7 +63178,7 @@
         <v>954</v>
       </c>
       <c r="G2448">
-        <v>0.764705882</v>
+        <v>0.764706</v>
       </c>
       <c r="H2448" t="s">
         <v>896</v>
@@ -63252,7 +63186,7 @@
     </row>
     <row r="2449" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2449" t="s">
-        <v>603</v>
+        <v>214</v>
       </c>
       <c r="B2449" t="s">
         <v>947</v>
@@ -63261,7 +63195,7 @@
         <v>948</v>
       </c>
       <c r="D2449" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2449" t="s">
         <v>955</v>
@@ -63270,7 +63204,7 @@
         <v>956</v>
       </c>
       <c r="G2449">
-        <v>0.70588235300000002</v>
+        <v>0.70588200000000001</v>
       </c>
       <c r="H2449" t="s">
         <v>896</v>
@@ -63278,7 +63212,7 @@
     </row>
     <row r="2450" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2450" t="s">
-        <v>681</v>
+        <v>214</v>
       </c>
       <c r="B2450" t="s">
         <v>947</v>
@@ -63287,7 +63221,7 @@
         <v>948</v>
       </c>
       <c r="D2450" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2450" t="s">
         <v>957</v>
@@ -63296,7 +63230,7 @@
         <v>958</v>
       </c>
       <c r="G2450">
-        <v>0.82352941199999996</v>
+        <v>0.82352899999999996</v>
       </c>
       <c r="H2450" t="s">
         <v>896</v>
@@ -63304,7 +63238,7 @@
     </row>
     <row r="2451" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2451" t="s">
-        <v>395</v>
+        <v>299</v>
       </c>
       <c r="B2451" t="s">
         <v>949</v>
@@ -63313,7 +63247,7 @@
         <v>950</v>
       </c>
       <c r="D2451" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="E2451" t="s">
         <v>951</v>
@@ -63322,15 +63256,12 @@
         <v>397</v>
       </c>
       <c r="G2451">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2451" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2452" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2452" t="s">
-        <v>480</v>
+        <v>299</v>
       </c>
       <c r="B2452" t="s">
         <v>949</v>
@@ -63339,7 +63270,7 @@
         <v>950</v>
       </c>
       <c r="D2452" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2452" t="s">
         <v>952</v>
@@ -63348,15 +63279,12 @@
         <v>482</v>
       </c>
       <c r="G2452">
-        <v>0.92307692299999999</v>
-      </c>
-      <c r="H2452" t="s">
-        <v>896</v>
+        <v>0.92307700000000004</v>
       </c>
     </row>
     <row r="2453" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2453" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
       <c r="B2453" t="s">
         <v>949</v>
@@ -63374,7 +63302,7 @@
         <v>954</v>
       </c>
       <c r="G2453">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2453" t="s">
         <v>896</v>
@@ -63382,7 +63310,7 @@
     </row>
     <row r="2454" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2454" t="s">
-        <v>603</v>
+        <v>299</v>
       </c>
       <c r="B2454" t="s">
         <v>949</v>
@@ -63391,7 +63319,7 @@
         <v>950</v>
       </c>
       <c r="D2454" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2454" t="s">
         <v>955</v>
@@ -63408,7 +63336,7 @@
     </row>
     <row r="2455" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2455" t="s">
-        <v>681</v>
+        <v>299</v>
       </c>
       <c r="B2455" t="s">
         <v>949</v>
@@ -63417,7 +63345,7 @@
         <v>950</v>
       </c>
       <c r="D2455" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2455" t="s">
         <v>957</v>
@@ -63434,7 +63362,7 @@
     </row>
     <row r="2456" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2456" t="s">
-        <v>480</v>
+        <v>395</v>
       </c>
       <c r="B2456" t="s">
         <v>951</v>
@@ -63443,7 +63371,7 @@
         <v>397</v>
       </c>
       <c r="D2456" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="E2456" t="s">
         <v>952</v>
@@ -63460,7 +63388,7 @@
     </row>
     <row r="2457" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2457" t="s">
-        <v>522</v>
+        <v>395</v>
       </c>
       <c r="B2457" t="s">
         <v>951</v>
@@ -63478,7 +63406,7 @@
         <v>954</v>
       </c>
       <c r="G2457">
-        <v>0.85714285700000004</v>
+        <v>0.85714299999999999</v>
       </c>
       <c r="H2457" t="s">
         <v>896</v>
@@ -63486,7 +63414,7 @@
     </row>
     <row r="2458" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2458" t="s">
-        <v>603</v>
+        <v>395</v>
       </c>
       <c r="B2458" t="s">
         <v>951</v>
@@ -63495,7 +63423,7 @@
         <v>397</v>
       </c>
       <c r="D2458" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2458" t="s">
         <v>955</v>
@@ -63512,7 +63440,7 @@
     </row>
     <row r="2459" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2459" t="s">
-        <v>681</v>
+        <v>395</v>
       </c>
       <c r="B2459" t="s">
         <v>951</v>
@@ -63521,7 +63449,7 @@
         <v>397</v>
       </c>
       <c r="D2459" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2459" t="s">
         <v>957</v>
@@ -63538,7 +63466,7 @@
     </row>
     <row r="2460" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2460" t="s">
-        <v>522</v>
+        <v>480</v>
       </c>
       <c r="B2460" t="s">
         <v>952</v>
@@ -63556,7 +63484,7 @@
         <v>954</v>
       </c>
       <c r="G2460">
-        <v>0.78571428600000004</v>
+        <v>0.78571400000000002</v>
       </c>
       <c r="H2460" t="s">
         <v>896</v>
@@ -63564,7 +63492,7 @@
     </row>
     <row r="2461" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2461" t="s">
-        <v>603</v>
+        <v>480</v>
       </c>
       <c r="B2461" t="s">
         <v>952</v>
@@ -63573,7 +63501,7 @@
         <v>482</v>
       </c>
       <c r="D2461" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2461" t="s">
         <v>955</v>
@@ -63590,7 +63518,7 @@
     </row>
     <row r="2462" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2462" t="s">
-        <v>681</v>
+        <v>480</v>
       </c>
       <c r="B2462" t="s">
         <v>952</v>
@@ -63599,7 +63527,7 @@
         <v>482</v>
       </c>
       <c r="D2462" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2462" t="s">
         <v>957</v>
@@ -63616,7 +63544,7 @@
     </row>
     <row r="2463" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2463" t="s">
-        <v>603</v>
+        <v>522</v>
       </c>
       <c r="B2463" t="s">
         <v>953</v>
@@ -63625,7 +63553,7 @@
         <v>954</v>
       </c>
       <c r="D2463" t="s">
-        <v>522</v>
+        <v>603</v>
       </c>
       <c r="E2463" t="s">
         <v>955</v>
@@ -63642,7 +63570,7 @@
     </row>
     <row r="2464" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2464" t="s">
-        <v>681</v>
+        <v>522</v>
       </c>
       <c r="B2464" t="s">
         <v>953</v>
@@ -63651,7 +63579,7 @@
         <v>954</v>
       </c>
       <c r="D2464" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2464" t="s">
         <v>957</v>
@@ -63668,7 +63596,7 @@
     </row>
     <row r="2465" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2465" t="s">
-        <v>681</v>
+        <v>603</v>
       </c>
       <c r="B2465" t="s">
         <v>955</v>
@@ -63677,7 +63605,7 @@
         <v>956</v>
       </c>
       <c r="D2465" t="s">
-        <v>522</v>
+        <v>681</v>
       </c>
       <c r="E2465" t="s">
         <v>957</v>

</xml_diff>